<commit_message>
stuff this is not required man, truly
</commit_message>
<xml_diff>
--- a/love-babbar-dsa/FINAL450.xlsx
+++ b/love-babbar-dsa/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\notes\love-babbar-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C9F31E-9C01-463F-83C9-E0EFABB37D38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1AD8E-E387-4176-B7CD-C8A0694890A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="945" windowWidth="27645" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="71" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="71" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2421,7 +2421,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2432,7 +2432,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
@@ -2454,7 +2454,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2553,7 +2553,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21">
@@ -2586,7 +2586,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="21">

</xml_diff>

<commit_message>
spiral traversal of matrix
</commit_message>
<xml_diff>
--- a/love-babbar-dsa/FINAL450.xlsx
+++ b/love-babbar-dsa/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\notes\love-babbar-dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA1AD8E-E387-4176-B7CD-C8A0694890A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EE5BFC-DD31-44F2-8FA2-5AC6EE60DAC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="945" windowWidth="27645" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="71" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="71" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2306,7 +2306,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">

</xml_diff>